<commit_message>
docker build for digitalocean
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fkolyadin/Desktop/rnd/model_approaches/development/irr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D10F9D-AE6B-8E4F-B8DA-2E54189E6DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3691F017-1508-8049-8A37-22B5BD2192C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13500" yWindow="1540" windowWidth="24300" windowHeight="18800" xr2:uid="{6C7AF6B3-1CC2-6448-8686-AA751821789D}"/>
+    <workbookView xWindow="-26980" yWindow="22100" windowWidth="24300" windowHeight="18800" xr2:uid="{6C7AF6B3-1CC2-6448-8686-AA751821789D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>irr</t>
   </si>
@@ -42,9 +42,6 @@
     <t>get front end from monitoring and load it to git</t>
   </si>
   <si>
-    <t>make sure monitoring turns on / update all packages</t>
-  </si>
-  <si>
     <t>redo irr for mortgages</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>my filter on button needs an alert that it may take a few seconds to load</t>
   </si>
   <si>
-    <t>fix api to pass in a list of numeric values</t>
-  </si>
-  <si>
     <t>create an api module that would generate the url</t>
   </si>
   <si>
@@ -100,16 +94,55 @@
   </si>
   <si>
     <t>fix apr calculation</t>
+  </si>
+  <si>
+    <t>completed</t>
+  </si>
+  <si>
+    <t>fix ratesheet table (remove useless space)</t>
+  </si>
+  <si>
+    <t>fix sorting on ratesheet table</t>
+  </si>
+  <si>
+    <t>create services/product segment</t>
+  </si>
+  <si>
+    <t>redesign front end using bootstrap potentially</t>
+  </si>
+  <si>
+    <t>download latest repo and have them run locaclly to make changes</t>
+  </si>
+  <si>
+    <t>figure out how to load repo's to digital ocean and consider CI/CD</t>
+  </si>
+  <si>
+    <t>rebuild front end with most recent packages / add to repo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -135,9 +168,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,15 +488,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73C79E3D-E1B0-3547-9FC3-CE8A271C4F2B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:H22"/>
+  <dimension ref="B2:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.1640625" customWidth="1"/>
     <col min="5" max="5" width="30.83203125" customWidth="1"/>
     <col min="7" max="7" width="62" bestFit="1" customWidth="1"/>
   </cols>
@@ -471,13 +506,13 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
@@ -485,19 +520,19 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
@@ -505,17 +540,17 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5">
         <f>F4+1</f>
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
@@ -526,112 +561,143 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6">
         <f t="shared" ref="F6" si="0">F5+1</f>
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
-        <v>3</v>
-      </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <f>F6+1</f>
+        <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <f>F7+1</f>
+        <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="F9">
-        <f>F6+1</f>
-        <v>4</v>
+        <f>F8+1</f>
+        <v>6</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="F10">
         <f>F9+1</f>
-        <v>5</v>
-      </c>
-      <c r="G10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="F11">
         <f>F10+1</f>
-        <v>6</v>
-      </c>
-      <c r="G11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="F12">
-        <f>F11+1</f>
-        <v>7</v>
-      </c>
-      <c r="G12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="F13">
-        <f>F12+1</f>
         <v>8</v>
-      </c>
-      <c r="G13" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="G15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C18" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="G18" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-    </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="G19" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G20" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="G21" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D22" s="1"/>
+      <c r="G22" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G23" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G24" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G25" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G26" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G27" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G28" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>